<commit_message>
Add correct FigS7/S8 code
Update to use correct column for survival analysis, and delete missing rows in datasets
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwwhite/R_work/Kimbro/Cages_NCE_manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A92E66-198E-9D4F-A934-AC00CA043414}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B0AB83-CF1F-5B47-A51C-026C19B19847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34540" yWindow="760" windowWidth="25380" windowHeight="10340" xr2:uid="{96C0CF60-EB3F-9046-89D3-90C245DD5192}"/>
+    <workbookView xWindow="600" yWindow="700" windowWidth="28240" windowHeight="17540" xr2:uid="{96C0CF60-EB3F-9046-89D3-90C245DD5192}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="126">
   <si>
     <t>harvest</t>
   </si>
@@ -408,12 +408,6 @@
   </si>
   <si>
     <t>Growth (mm) of oysters during the experiment</t>
-  </si>
-  <si>
-    <t>waterht</t>
-  </si>
-  <si>
-    <t>average water depth recorded over experiment at each site</t>
   </si>
   <si>
     <t>Growth rate (mm/day) of oysters during the experiment (note that total deployment time was 77 days for some cages and 128 days for others)</t>
@@ -778,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{875B9D68-CCAA-4243-A047-6AE52E21F2CD}">
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="A158" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2101,234 +2095,212 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B140" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>77</v>
+        <v>105</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="B141" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B142" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="B143" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B144" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>119</v>
-      </c>
-      <c r="B145" t="s">
-        <v>117</v>
-      </c>
-      <c r="C145" s="1" t="s">
         <v>107</v>
       </c>
     </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B146" t="s">
+        <v>122</v>
+      </c>
+    </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B147" t="s">
-        <v>122</v>
+      <c r="A147" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="B148" t="s">
+        <v>2</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B150" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B151" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>110</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B152" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B153" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B154" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B155" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B156" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B157" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B158" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B159" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B160" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" t="s">
-        <v>53</v>
-      </c>
-      <c r="B161" t="s">
-        <v>116</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" t="s">
-        <v>82</v>
-      </c>
-      <c r="B162" t="s">
-        <v>117</v>
-      </c>
-      <c r="C162" s="1" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>